<commit_message>
Classification results 0-100 int
</commit_message>
<xml_diff>
--- a/BayesClassification/results/det_int_30.xlsx
+++ b/BayesClassification/results/det_int_30.xlsx
@@ -34,529 +34,529 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">2018-06-29 16:50:34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:50:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:50:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:51:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:51:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:51:24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:51:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:51:48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:51:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:52:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:52:19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:52:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:52:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:52:51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:53:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:53:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:53:24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:53:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:53:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:53:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:54:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:54:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:54:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:54:35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:54:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:54:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:55:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:55:21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:55:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:55:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:55:48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:56:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:56:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:56:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:56:32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:56:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:56:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:57:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:57:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:57:24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:57:35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:57:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:57:53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:58:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:58:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:58:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:58:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:58:47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:59:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:59:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:59:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:59:34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:59:42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 16:59:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:00:03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:00:12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:00:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:00:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:00:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:00:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:01:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:01:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:01:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:01:34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:01:42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:01:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:02:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:02:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:02:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:02:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:02:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:02:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:03:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:03:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:03:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:03:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:03:49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:04:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:04:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:04:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:04:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:04:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:04:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:05:02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:05:12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:05:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:05:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:05:42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:05:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:06:08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:06:14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:06:25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:06:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:06:47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:06:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:07:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:07:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:07:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:07:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:07:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:08:02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:08:11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:08:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:08:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:08:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:08:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:09:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:09:14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:09:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:09:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:09:47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:09:57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:10:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:10:19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:10:29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:10:41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:10:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:11:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:11:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:11:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:11:37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:11:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:11:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:12:08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:12:21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:12:29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:12:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:12:51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:13:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:13:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:13:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:13:37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:13:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:13:52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:14:03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:14:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:14:25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:14:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:14:47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:14:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:15:08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:15:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:15:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:15:41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:15:49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:16:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:16:11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:16:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:16:29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:16:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:16:49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:17:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:17:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:17:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:17:35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:17:47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:17:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:18:03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:18:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:18:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:18:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:18:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:18:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:19:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:19:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:19:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:19:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:19:51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:20:03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:20:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:20:21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:20:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:20:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:20:55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-06-29 17:21:06</t>
+    <t xml:space="preserve">2018-06-29 17:24:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:24:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:25:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:25:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:25:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:25:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:25:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:25:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:26:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:26:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:26:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:26:39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:26:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:27:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:27:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:27:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:27:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:27:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:27:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:27:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:28:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:28:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:28:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:28:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:28:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:29:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:29:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:29:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:29:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:29:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:29:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:30:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:30:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:30:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:30:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:30:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:31:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:31:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:31:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:31:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:31:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:32:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:32:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:32:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:32:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:32:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:32:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:32:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:33:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:33:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:33:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:33:39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:33:49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:33:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:34:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:34:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:34:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:34:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:34:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:35:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:35:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:35:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:35:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:35:39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:35:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:36:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:36:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:36:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:36:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:36:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:36:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:37:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:37:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:37:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:37:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:37:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:38:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:38:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:38:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:38:37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:38:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:38:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:39:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:39:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:39:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:39:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:39:49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:40:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:40:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:40:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:40:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:40:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:40:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:41:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:41:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:41:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:41:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:41:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:41:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:42:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:42:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:42:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:42:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:42:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:43:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:43:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:43:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:43:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:43:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:43:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:44:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:44:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:44:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:44:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:44:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:44:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:44:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:45:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:45:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:45:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:45:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:45:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:45:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:46:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:46:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:46:32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:46:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:46:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:47:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:47:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:47:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:47:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:47:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:47:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:48:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:48:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:48:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:48:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:48:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:48:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:49:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:49:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:49:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:49:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:49:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:50:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:50:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:50:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:50:37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:50:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:50:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:51:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:51:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:51:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:51:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:51:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:51:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:52:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:52:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:52:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:52:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:52:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:52:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:53:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:53:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:53:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:53:32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:53:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:53:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:54:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:54:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:54:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:54:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:54:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06-29 17:54:56</t>
   </si>
 </sst>
 </file>
@@ -789,10 +789,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -817,10 +817,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -831,10 +831,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>14</v>
@@ -845,10 +845,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>15</v>
@@ -859,10 +859,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -873,10 +873,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
@@ -887,10 +887,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
@@ -901,10 +901,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
@@ -915,10 +915,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>20</v>
@@ -929,10 +929,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>21</v>
@@ -943,10 +943,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>22</v>
@@ -957,10 +957,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>23</v>
@@ -971,10 +971,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>24</v>
@@ -1363,10 +1363,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>52</v>
@@ -1377,10 +1377,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>53</v>
@@ -1391,10 +1391,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>54</v>
@@ -1405,10 +1405,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>55</v>
@@ -1419,10 +1419,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>56</v>
@@ -1433,10 +1433,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>57</v>
@@ -1461,10 +1461,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>59</v>
@@ -1601,10 +1601,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>69</v>
@@ -1685,10 +1685,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>75</v>
@@ -1699,10 +1699,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>76</v>
@@ -1713,10 +1713,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>77</v>
@@ -1727,10 +1727,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>78</v>
@@ -1741,10 +1741,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>79</v>
@@ -1755,10 +1755,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>80</v>
@@ -1769,10 +1769,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>81</v>
@@ -1783,10 +1783,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>82</v>
@@ -1797,10 +1797,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>83</v>
@@ -1811,10 +1811,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>84</v>
@@ -1825,10 +1825,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>85</v>
@@ -1839,10 +1839,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>86</v>
@@ -1853,10 +1853,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>87</v>
@@ -1895,10 +1895,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>90</v>
@@ -1909,10 +1909,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>91</v>
@@ -1923,10 +1923,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>92</v>
@@ -2175,10 +2175,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C108" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>110</v>
@@ -2189,10 +2189,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C109" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>111</v>
@@ -2203,10 +2203,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C110" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>112</v>
@@ -2217,10 +2217,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C111" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>113</v>
@@ -2231,10 +2231,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C112" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>114</v>
@@ -2413,10 +2413,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C125" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>127</v>
@@ -2427,10 +2427,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C126" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>128</v>
@@ -2441,10 +2441,10 @@
         <v>126</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C127" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>129</v>
@@ -2455,10 +2455,10 @@
         <v>127</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C128" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>130</v>
@@ -2469,10 +2469,10 @@
         <v>128</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C129" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>131</v>
@@ -2497,10 +2497,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C131" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>133</v>
@@ -2511,10 +2511,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C132" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>134</v>
@@ -2525,10 +2525,10 @@
         <v>132</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C133" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>135</v>
@@ -2539,10 +2539,10 @@
         <v>133</v>
       </c>
       <c r="B134" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C134" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>136</v>
@@ -2553,10 +2553,10 @@
         <v>134</v>
       </c>
       <c r="B135" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C135" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>137</v>
@@ -2567,10 +2567,10 @@
         <v>135</v>
       </c>
       <c r="B136" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C136" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>138</v>
@@ -2581,10 +2581,10 @@
         <v>136</v>
       </c>
       <c r="B137" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C137" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>139</v>
@@ -2595,10 +2595,10 @@
         <v>137</v>
       </c>
       <c r="B138" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C138" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>140</v>
@@ -2609,10 +2609,10 @@
         <v>138</v>
       </c>
       <c r="B139" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C139" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>141</v>
@@ -2623,10 +2623,10 @@
         <v>139</v>
       </c>
       <c r="B140" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C140" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>142</v>
@@ -2637,10 +2637,10 @@
         <v>140</v>
       </c>
       <c r="B141" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C141" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>143</v>
@@ -2651,10 +2651,10 @@
         <v>141</v>
       </c>
       <c r="B142" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C142" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>144</v>
@@ -2665,10 +2665,10 @@
         <v>142</v>
       </c>
       <c r="B143" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C143" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>145</v>
@@ -2679,10 +2679,10 @@
         <v>143</v>
       </c>
       <c r="B144" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C144" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>146</v>
@@ -2707,10 +2707,10 @@
         <v>145</v>
       </c>
       <c r="B146" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C146" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>148</v>
@@ -2721,10 +2721,10 @@
         <v>146</v>
       </c>
       <c r="B147" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C147" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>149</v>
@@ -2735,10 +2735,10 @@
         <v>147</v>
       </c>
       <c r="B148" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C148" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>150</v>
@@ -2749,10 +2749,10 @@
         <v>148</v>
       </c>
       <c r="B149" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C149" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>151</v>
@@ -2763,10 +2763,10 @@
         <v>149</v>
       </c>
       <c r="B150" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C150" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>152</v>
@@ -2791,10 +2791,10 @@
         <v>151</v>
       </c>
       <c r="B152" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C152" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>154</v>
@@ -2819,10 +2819,10 @@
         <v>153</v>
       </c>
       <c r="B154" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C154" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>156</v>
@@ -2833,10 +2833,10 @@
         <v>154</v>
       </c>
       <c r="B155" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C155" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>157</v>
@@ -2847,10 +2847,10 @@
         <v>155</v>
       </c>
       <c r="B156" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C156" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>158</v>
@@ -2861,10 +2861,10 @@
         <v>156</v>
       </c>
       <c r="B157" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C157" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>159</v>
@@ -2875,10 +2875,10 @@
         <v>157</v>
       </c>
       <c r="B158" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C158" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>160</v>
@@ -2889,10 +2889,10 @@
         <v>158</v>
       </c>
       <c r="B159" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C159" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>161</v>
@@ -2903,10 +2903,10 @@
         <v>159</v>
       </c>
       <c r="B160" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C160" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>162</v>
@@ -2917,10 +2917,10 @@
         <v>160</v>
       </c>
       <c r="B161" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C161" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>163</v>
@@ -2931,10 +2931,10 @@
         <v>161</v>
       </c>
       <c r="B162" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C162" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>164</v>
@@ -2945,10 +2945,10 @@
         <v>162</v>
       </c>
       <c r="B163" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C163" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>165</v>
@@ -2959,10 +2959,10 @@
         <v>163</v>
       </c>
       <c r="B164" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C164" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>166</v>
@@ -2987,10 +2987,10 @@
         <v>165</v>
       </c>
       <c r="B166" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C166" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>168</v>
@@ -3001,10 +3001,10 @@
         <v>166</v>
       </c>
       <c r="B167" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C167" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>169</v>
@@ -3057,10 +3057,10 @@
         <v>170</v>
       </c>
       <c r="B171" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C171" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>173</v>
@@ -3071,10 +3071,10 @@
         <v>171</v>
       </c>
       <c r="B172" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C172" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>174</v>
@@ -3085,10 +3085,10 @@
         <v>172</v>
       </c>
       <c r="B173" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C173" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>175</v>
@@ -3099,10 +3099,10 @@
         <v>173</v>
       </c>
       <c r="B174" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C174" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>176</v>
@@ -3113,10 +3113,10 @@
         <v>174</v>
       </c>
       <c r="B175" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C175" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>177</v>
@@ -3127,10 +3127,10 @@
         <v>175</v>
       </c>
       <c r="B176" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C176" s="0" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>178</v>

</xml_diff>